<commit_message>
fixed row / col confusion - vol surface still looks off
</commit_message>
<xml_diff>
--- a/Data/ArtificialPriceData.xlsx
+++ b/Data/ArtificialPriceData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\source\repos\QuantFinance\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7F0A2A0-1D06-4E76-B5BB-42B4AFDD1172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1778D7CD-D962-4292-813F-16DBC6218049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1090" yWindow="2320" windowWidth="18760" windowHeight="10550" xr2:uid="{F36D0F92-47DA-4F50-B766-681428CA8F76}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="18760" windowHeight="10550" activeTab="1" xr2:uid="{F36D0F92-47DA-4F50-B766-681428CA8F76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="330">
   <si>
     <t>Strike \ Expiry (weeks)</t>
   </si>
@@ -648,6 +649,384 @@
   </si>
   <si>
     <t>6.55</t>
+  </si>
+  <si>
+    <t>Expiry (weeks)</t>
+  </si>
+  <si>
+    <t>25.10</t>
+  </si>
+  <si>
+    <t>23.15</t>
+  </si>
+  <si>
+    <t>21.25</t>
+  </si>
+  <si>
+    <t>19.40</t>
+  </si>
+  <si>
+    <t>17.60</t>
+  </si>
+  <si>
+    <t>15.85</t>
+  </si>
+  <si>
+    <t>14.15</t>
+  </si>
+  <si>
+    <t>10.90</t>
+  </si>
+  <si>
+    <t>9.35</t>
+  </si>
+  <si>
+    <t>6.40</t>
+  </si>
+  <si>
+    <t>3.65</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>24.10</t>
+  </si>
+  <si>
+    <t>22.25</t>
+  </si>
+  <si>
+    <t>20.45</t>
+  </si>
+  <si>
+    <t>18.70</t>
+  </si>
+  <si>
+    <t>15.35</t>
+  </si>
+  <si>
+    <t>13.75</t>
+  </si>
+  <si>
+    <t>12.20</t>
+  </si>
+  <si>
+    <t>10.70</t>
+  </si>
+  <si>
+    <t>9.25</t>
+  </si>
+  <si>
+    <t>3.95</t>
+  </si>
+  <si>
+    <t>2.75</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.70</t>
+  </si>
+  <si>
+    <t>26.90</t>
+  </si>
+  <si>
+    <t>25.05</t>
+  </si>
+  <si>
+    <t>19.80</t>
+  </si>
+  <si>
+    <t>18.15</t>
+  </si>
+  <si>
+    <t>16.55</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>13.50</t>
+  </si>
+  <si>
+    <t>10.65</t>
+  </si>
+  <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>5.55</t>
+  </si>
+  <si>
+    <t>3.30</t>
+  </si>
+  <si>
+    <t>2.30</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>27.75</t>
+  </si>
+  <si>
+    <t>25.95</t>
+  </si>
+  <si>
+    <t>24.20</t>
+  </si>
+  <si>
+    <t>20.85</t>
+  </si>
+  <si>
+    <t>19.25</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>9.45</t>
+  </si>
+  <si>
+    <t>8.25</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>2.80</t>
+  </si>
+  <si>
+    <t>28.55</t>
+  </si>
+  <si>
+    <t>26.80</t>
+  </si>
+  <si>
+    <t>23.40</t>
+  </si>
+  <si>
+    <t>21.80</t>
+  </si>
+  <si>
+    <t>20.25</t>
+  </si>
+  <si>
+    <t>18.75</t>
+  </si>
+  <si>
+    <t>15.90</t>
+  </si>
+  <si>
+    <t>14.55</t>
+  </si>
+  <si>
+    <t>13.25</t>
+  </si>
+  <si>
+    <t>10.80</t>
+  </si>
+  <si>
+    <t>9.65</t>
+  </si>
+  <si>
+    <t>7.50</t>
+  </si>
+  <si>
+    <t>4.85</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>29.30</t>
+  </si>
+  <si>
+    <t>25.90</t>
+  </si>
+  <si>
+    <t>24.25</t>
+  </si>
+  <si>
+    <t>22.70</t>
+  </si>
+  <si>
+    <t>21.20</t>
+  </si>
+  <si>
+    <t>19.75</t>
+  </si>
+  <si>
+    <t>14.45</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>9.95</t>
+  </si>
+  <si>
+    <t>8.95</t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>28.35</t>
+  </si>
+  <si>
+    <t>26.65</t>
+  </si>
+  <si>
+    <t>22.10</t>
+  </si>
+  <si>
+    <t>20.70</t>
+  </si>
+  <si>
+    <t>19.35</t>
+  </si>
+  <si>
+    <t>18.05</t>
+  </si>
+  <si>
+    <t>16.80</t>
+  </si>
+  <si>
+    <t>11.30</t>
+  </si>
+  <si>
+    <t>10.35</t>
+  </si>
+  <si>
+    <t>8.60</t>
+  </si>
+  <si>
+    <t>30.65</t>
+  </si>
+  <si>
+    <t>29.05</t>
+  </si>
+  <si>
+    <t>27.35</t>
+  </si>
+  <si>
+    <t>24.30</t>
+  </si>
+  <si>
+    <t>22.90</t>
+  </si>
+  <si>
+    <t>21.55</t>
+  </si>
+  <si>
+    <t>19.00</t>
+  </si>
+  <si>
+    <t>17.80</t>
+  </si>
+  <si>
+    <t>15.55</t>
+  </si>
+  <si>
+    <t>14.50</t>
+  </si>
+  <si>
+    <t>12.55</t>
+  </si>
+  <si>
+    <t>11.65</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>8.65</t>
+  </si>
+  <si>
+    <t>31.25</t>
+  </si>
+  <si>
+    <t>29.70</t>
+  </si>
+  <si>
+    <t>26.40</t>
+  </si>
+  <si>
+    <t>23.60</t>
+  </si>
+  <si>
+    <t>22.30</t>
+  </si>
+  <si>
+    <t>19.85</t>
+  </si>
+  <si>
+    <t>14.60</t>
+  </si>
+  <si>
+    <t>13.70</t>
+  </si>
+  <si>
+    <t>12.85</t>
+  </si>
+  <si>
+    <t>10.60</t>
+  </si>
+  <si>
+    <t>31.80</t>
+  </si>
+  <si>
+    <t>30.30</t>
+  </si>
+  <si>
+    <t>27.00</t>
+  </si>
+  <si>
+    <t>20.65</t>
+  </si>
+  <si>
+    <t>19.55</t>
+  </si>
+  <si>
+    <t>17.50</t>
+  </si>
+  <si>
+    <t>15.65</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3822464B-A0DC-4C5A-98C5-92A7E4F691F8}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1814,4 +2193,767 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DE3BEB-1258-4415-938A-AA07684CA2F2}">
+  <dimension ref="A1:V11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="1">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1">
+        <v>155</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1">
+        <v>160</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1">
+        <v>165</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="1">
+        <v>170</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="1">
+        <v>175</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="1">
+        <v>180</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P1" s="1">
+        <v>185</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="R1" s="1">
+        <v>190</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" s="1">
+        <v>195</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="V1" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>